<commit_message>
update operation of stock
</commit_message>
<xml_diff>
--- a/storage/account.xlsx
+++ b/storage/account.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>id</t>
   </si>
@@ -56,7 +56,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>Oct 29, 2023</t>
+    <t>Dec 4, 2023</t>
   </si>
   <si>
     <t>الخصوم</t>
@@ -74,10 +74,217 @@
     <t>الاصول المتداوله</t>
   </si>
   <si>
+    <t>الخصوم الثابته</t>
+  </si>
+  <si>
+    <t>الخصوم المتداوله</t>
+  </si>
+  <si>
+    <t>حسابات داينه اخري</t>
+  </si>
+  <si>
+    <t>المبيعات</t>
+  </si>
+  <si>
+    <t>ايرادات حضور وغياب</t>
+  </si>
+  <si>
+    <t>Mar 5, 2024</t>
+  </si>
+  <si>
+    <t>مصروف رواتب واجور</t>
+  </si>
+  <si>
+    <t>مصروفات اداريه</t>
+  </si>
+  <si>
+    <t>مصروفات عموميه</t>
+  </si>
+  <si>
+    <t>مصروفات نثريه</t>
+  </si>
+  <si>
+    <t>مصروفات اخري</t>
+  </si>
+  <si>
+    <t>الاراضي</t>
+  </si>
+  <si>
+    <t>السيارات</t>
+  </si>
+  <si>
+    <t>العقارات</t>
+  </si>
+  <si>
+    <t>البنك</t>
+  </si>
+  <si>
     <t>الصندوق</t>
   </si>
   <si>
-    <t>البنك</t>
+    <t>العملاء المدينون</t>
+  </si>
+  <si>
+    <t>المخزون</t>
+  </si>
+  <si>
+    <t>سلف الموظفين</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>خصميات الموظف</t>
+  </si>
+  <si>
+    <t>Feb 23, 2024</t>
+  </si>
+  <si>
+    <t>الموردون الداينون</t>
+  </si>
+  <si>
+    <t>مستحقات الموظفين</t>
+  </si>
+  <si>
+    <t>اضافي الموظف</t>
+  </si>
+  <si>
+    <t>بدلات الموظف</t>
+  </si>
+  <si>
+    <t>ايرادات غياب</t>
+  </si>
+  <si>
+    <t>ايرادات تأخير</t>
+  </si>
+  <si>
+    <t>ايرادات انصراف مبكر</t>
+  </si>
+  <si>
+    <t>ايرادات خصم اخري</t>
+  </si>
+  <si>
+    <t>مصروف الرواتب</t>
+  </si>
+  <si>
+    <t>Feb 24, 2024</t>
+  </si>
+  <si>
+    <t>مصروف البدلات</t>
+  </si>
+  <si>
+    <t>مصروف الاضافي</t>
+  </si>
+  <si>
+    <t>فواتير كهرباء</t>
+  </si>
+  <si>
+    <t>Dec 12, 2023</t>
+  </si>
+  <si>
+    <t>فواتير ماء</t>
+  </si>
+  <si>
+    <t>فواتير هاتف</t>
+  </si>
+  <si>
+    <t>صدقات وتبرعات</t>
+  </si>
+  <si>
+    <t>May 4, 2024</t>
+  </si>
+  <si>
+    <t>بنك الكريمي</t>
+  </si>
+  <si>
+    <t>Dec 5, 2023</t>
+  </si>
+  <si>
+    <t>بنك دولار</t>
+  </si>
+  <si>
+    <t>Mar 31, 2024</t>
+  </si>
+  <si>
+    <t>صندوق حده المدينه</t>
+  </si>
+  <si>
+    <t>صندوق باب اليمن</t>
+  </si>
+  <si>
+    <t>صندوق دولار</t>
+  </si>
+  <si>
+    <t>صندوق ريال</t>
+  </si>
+  <si>
+    <t>العميل محمد علي حسن</t>
+  </si>
+  <si>
+    <t>عملاء تعز</t>
+  </si>
+  <si>
+    <t>Mar 30, 2024</t>
+  </si>
+  <si>
+    <t>عملاء صنعاء</t>
+  </si>
+  <si>
+    <t>المخزن الريسي</t>
+  </si>
+  <si>
+    <t>المخزن المركزي الاول</t>
+  </si>
+  <si>
+    <t>مخزن المواد الغذائيه</t>
+  </si>
+  <si>
+    <t>Apr 8, 2024</t>
+  </si>
+  <si>
+    <t>غياب</t>
+  </si>
+  <si>
+    <t>تأخير</t>
+  </si>
+  <si>
+    <t>انصراف مبكر</t>
+  </si>
+  <si>
+    <t>خصميات اخري</t>
+  </si>
+  <si>
+    <t>المورد مهيب احمد عبدالجليل الجنيد الجنيد</t>
+  </si>
+  <si>
+    <t>موردين تعز</t>
+  </si>
+  <si>
+    <t>موردين صنعاء</t>
+  </si>
+  <si>
+    <t>بدل مواصلات</t>
+  </si>
+  <si>
+    <t>May 13, 2024</t>
+  </si>
+  <si>
+    <t>بدل سكن</t>
+  </si>
+  <si>
+    <t>بدل تغذيه</t>
+  </si>
+  <si>
+    <t>مصروف بدلات السكن</t>
+  </si>
+  <si>
+    <t>Feb 26, 2024</t>
+  </si>
+  <si>
+    <t>مصروف بدلات المواصلات</t>
+  </si>
+  <si>
+    <t>مصروف بدلات التغذيه</t>
   </si>
 </sst>
 </file>
@@ -417,7 +624,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,16 +783,16 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
         <v>12</v>
@@ -599,16 +806,16 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9" t="s">
         <v>12</v>
@@ -618,6 +825,1317 @@
       </c>
       <c r="K9" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>112</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="I19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>122</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>123</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>124</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>125</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>126</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>221</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <v>231</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28">
+        <v>23</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>232</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29">
+        <v>23</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>38</v>
+      </c>
+      <c r="J29" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <v>233</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30">
+        <v>23</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>38</v>
+      </c>
+      <c r="J30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31">
+        <v>321</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31">
+        <v>32</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="I31" t="s">
+        <v>38</v>
+      </c>
+      <c r="J31" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32">
+        <v>322</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32">
+        <v>32</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="I32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33">
+        <v>323</v>
+      </c>
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>38</v>
+      </c>
+      <c r="J33" t="s">
+        <v>24</v>
+      </c>
+      <c r="K33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34">
+        <v>324</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34">
+        <v>32</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="I34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J34" t="s">
+        <v>24</v>
+      </c>
+      <c r="K34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <v>411</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35">
+        <v>41</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="I35" t="s">
+        <v>38</v>
+      </c>
+      <c r="J35" t="s">
+        <v>50</v>
+      </c>
+      <c r="K35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36">
+        <v>412</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36">
+        <v>41</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="I36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J36" t="s">
+        <v>50</v>
+      </c>
+      <c r="K36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37">
+        <v>413</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37">
+        <v>41</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J37" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38">
+        <v>441</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38">
+        <v>44</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="I38" t="s">
+        <v>38</v>
+      </c>
+      <c r="J38" t="s">
+        <v>54</v>
+      </c>
+      <c r="K38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39">
+        <v>442</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39">
+        <v>44</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="I39" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" t="s">
+        <v>54</v>
+      </c>
+      <c r="K39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40">
+        <v>443</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40">
+        <v>44</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="I40" t="s">
+        <v>38</v>
+      </c>
+      <c r="J40" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41">
+        <v>451</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41">
+        <v>45</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="I41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J41" t="s">
+        <v>58</v>
+      </c>
+      <c r="K41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42">
+        <v>1211</v>
+      </c>
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42">
+        <v>121</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="I42" t="s">
+        <v>38</v>
+      </c>
+      <c r="J42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43">
+        <v>1212</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43">
+        <v>121</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>38</v>
+      </c>
+      <c r="J43" t="s">
+        <v>62</v>
+      </c>
+      <c r="K43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44">
+        <v>1221</v>
+      </c>
+      <c r="B44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44">
+        <v>122</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" t="s">
+        <v>60</v>
+      </c>
+      <c r="K44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45">
+        <v>1222</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45">
+        <v>122</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="I45" t="s">
+        <v>38</v>
+      </c>
+      <c r="J45" t="s">
+        <v>60</v>
+      </c>
+      <c r="K45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46">
+        <v>1223</v>
+      </c>
+      <c r="B46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46">
+        <v>122</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="I46" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" t="s">
+        <v>62</v>
+      </c>
+      <c r="K46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47">
+        <v>1224</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47">
+        <v>122</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="I47" t="s">
+        <v>38</v>
+      </c>
+      <c r="J47" t="s">
+        <v>62</v>
+      </c>
+      <c r="K47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48">
+        <v>1231</v>
+      </c>
+      <c r="B48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48">
+        <v>123</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="I48" t="s">
+        <v>38</v>
+      </c>
+      <c r="J48" t="s">
+        <v>60</v>
+      </c>
+      <c r="K48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49">
+        <v>1232</v>
+      </c>
+      <c r="B49" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49">
+        <v>123</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>38</v>
+      </c>
+      <c r="J49" t="s">
+        <v>69</v>
+      </c>
+      <c r="K49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50">
+        <v>1233</v>
+      </c>
+      <c r="B50" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50">
+        <v>123</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="I50" t="s">
+        <v>38</v>
+      </c>
+      <c r="J50" t="s">
+        <v>69</v>
+      </c>
+      <c r="K50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51">
+        <v>1241</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51">
+        <v>124</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="I51" t="s">
+        <v>38</v>
+      </c>
+      <c r="J51" t="s">
+        <v>60</v>
+      </c>
+      <c r="K51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52">
+        <v>1242</v>
+      </c>
+      <c r="B52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52">
+        <v>124</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="I52" t="s">
+        <v>38</v>
+      </c>
+      <c r="J52" t="s">
+        <v>60</v>
+      </c>
+      <c r="K52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53">
+        <v>1243</v>
+      </c>
+      <c r="B53" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53">
+        <v>124</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="I53" t="s">
+        <v>38</v>
+      </c>
+      <c r="J53" t="s">
+        <v>74</v>
+      </c>
+      <c r="K53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54">
+        <v>1261</v>
+      </c>
+      <c r="B54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54">
+        <v>126</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="I54" t="s">
+        <v>38</v>
+      </c>
+      <c r="J54" t="s">
+        <v>50</v>
+      </c>
+      <c r="K54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55">
+        <v>1262</v>
+      </c>
+      <c r="B55" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55">
+        <v>126</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="I55" t="s">
+        <v>38</v>
+      </c>
+      <c r="J55" t="s">
+        <v>50</v>
+      </c>
+      <c r="K55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56">
+        <v>1263</v>
+      </c>
+      <c r="B56" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56">
+        <v>126</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="I56" t="s">
+        <v>38</v>
+      </c>
+      <c r="J56" t="s">
+        <v>50</v>
+      </c>
+      <c r="K56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57">
+        <v>1264</v>
+      </c>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57">
+        <v>126</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="I57" t="s">
+        <v>38</v>
+      </c>
+      <c r="J57" t="s">
+        <v>50</v>
+      </c>
+      <c r="K57" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58">
+        <v>2211</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58">
+        <v>221</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="I58" t="s">
+        <v>38</v>
+      </c>
+      <c r="J58" t="s">
+        <v>60</v>
+      </c>
+      <c r="K58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59">
+        <v>2212</v>
+      </c>
+      <c r="B59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59">
+        <v>221</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+      <c r="I59" t="s">
+        <v>38</v>
+      </c>
+      <c r="J59" t="s">
+        <v>69</v>
+      </c>
+      <c r="K59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60">
+        <v>2213</v>
+      </c>
+      <c r="B60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60">
+        <v>221</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="I60" t="s">
+        <v>38</v>
+      </c>
+      <c r="J60" t="s">
+        <v>69</v>
+      </c>
+      <c r="K60" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61">
+        <v>2331</v>
+      </c>
+      <c r="B61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61">
+        <v>233</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="I61" t="s">
+        <v>38</v>
+      </c>
+      <c r="J61" t="s">
+        <v>83</v>
+      </c>
+      <c r="K61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62">
+        <v>2332</v>
+      </c>
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62">
+        <v>233</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="I62" t="s">
+        <v>38</v>
+      </c>
+      <c r="J62" t="s">
+        <v>83</v>
+      </c>
+      <c r="K62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63">
+        <v>2333</v>
+      </c>
+      <c r="B63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63">
+        <v>233</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="I63" t="s">
+        <v>38</v>
+      </c>
+      <c r="J63" t="s">
+        <v>83</v>
+      </c>
+      <c r="K63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64">
+        <v>4121</v>
+      </c>
+      <c r="B64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64">
+        <v>412</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="I64" t="s">
+        <v>38</v>
+      </c>
+      <c r="J64" t="s">
+        <v>87</v>
+      </c>
+      <c r="K64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65">
+        <v>4122</v>
+      </c>
+      <c r="B65" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65">
+        <v>412</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="I65" t="s">
+        <v>38</v>
+      </c>
+      <c r="J65" t="s">
+        <v>87</v>
+      </c>
+      <c r="K65" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66">
+        <v>4123</v>
+      </c>
+      <c r="B66" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66">
+        <v>412</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="I66" t="s">
+        <v>38</v>
+      </c>
+      <c r="J66" t="s">
+        <v>87</v>
+      </c>
+      <c r="K66" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>